<commit_message>
adding more data for Q&A
</commit_message>
<xml_diff>
--- a/progress_tracking.xlsx
+++ b/progress_tracking.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmymalhan/Documents/coding_interview_questions_with_python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7043CF41-F7A8-A345-8B1E-93580B7ADE74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF184944-1D79-7C40-8EBD-17BFF230C824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23480" yWindow="460" windowWidth="14720" windowHeight="19460" xr2:uid="{F06102A6-E2EC-1D48-A39E-FADE5E4F08CB}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19460" xr2:uid="{F06102A6-E2EC-1D48-A39E-FADE5E4F08CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction to Python" sheetId="1" r:id="rId1"/>
-    <sheet name="Daily Problems" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
   <si>
     <t>Introduction</t>
   </si>
@@ -100,6 +99,9 @@
   </si>
   <si>
     <t>Good</t>
+  </si>
+  <si>
+    <t>#Don't touch Medium Questions yet</t>
   </si>
 </sst>
 </file>
@@ -462,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F12CB8-A19F-CC45-8D69-91F1548814D1}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -475,9 +477,10 @@
     <col min="3" max="3" width="19.83203125" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
     <col min="5" max="5" width="34" customWidth="1"/>
+    <col min="6" max="6" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -493,8 +496,11 @@
       <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44145</v>
       </c>
@@ -511,7 +517,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>44144</v>
       </c>
@@ -528,7 +534,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>44144</v>
       </c>
@@ -542,10 +548,10 @@
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>44144</v>
       </c>
@@ -562,7 +568,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44144</v>
       </c>
@@ -576,10 +582,10 @@
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44144</v>
       </c>
@@ -596,22 +602,22 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>44144</v>
       </c>
@@ -628,7 +634,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>44144</v>
       </c>
@@ -645,7 +651,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44144</v>
       </c>
@@ -665,25 +671,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B499FF1A-2C2F-EE4D-AD7C-74590744698B}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="A1:F13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
commit with a plan
</commit_message>
<xml_diff>
--- a/progress_tracking.xlsx
+++ b/progress_tracking.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmymalhan/Documents/code_master_platform/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2690E2B5-6CF8-6540-A032-56DF60C02F39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889A4505-054D-1E43-AB77-8AE4FF4EC4F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41380" yWindow="840" windowWidth="33600" windowHeight="18860" xr2:uid="{F06102A6-E2EC-1D48-A39E-FADE5E4F08CB}"/>
+    <workbookView xWindow="3860" yWindow="1040" windowWidth="33600" windowHeight="18860" xr2:uid="{F06102A6-E2EC-1D48-A39E-FADE5E4F08CB}"/>
   </bookViews>
   <sheets>
     <sheet name="30 Days of Code" sheetId="2" r:id="rId1"/>
-    <sheet name="Problem Solving - Easy" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
   <si>
     <t>Introduction</t>
   </si>
@@ -63,18 +62,6 @@
     <t>Write a function</t>
   </si>
   <si>
-    <t>Leet Code</t>
-  </si>
-  <si>
-    <t>Fibonacci</t>
-  </si>
-  <si>
-    <t>Binary Search</t>
-  </si>
-  <si>
-    <t>Two Sum</t>
-  </si>
-  <si>
     <t>Date Attempted</t>
   </si>
   <si>
@@ -90,18 +77,12 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>Algo Expert</t>
-  </si>
-  <si>
     <t>Try Again</t>
   </si>
   <si>
     <t>Good</t>
   </si>
   <si>
-    <t>#Don't touch Medium Questions yet</t>
-  </si>
-  <si>
     <t>Introduction to Python</t>
   </si>
   <si>
@@ -111,9 +92,6 @@
     <t>Data Types</t>
   </si>
   <si>
-    <t>naive approach</t>
-  </si>
-  <si>
     <t>Hello World</t>
   </si>
   <si>
@@ -133,13 +111,52 @@
   </si>
   <si>
     <t>almost got it</t>
+  </si>
+  <si>
+    <t>Compare the triplets</t>
+  </si>
+  <si>
+    <t>Found Nice solution</t>
+  </si>
+  <si>
+    <t>Context for Hacker Rank</t>
+  </si>
+  <si>
+    <t>Planning till November 15</t>
+  </si>
+  <si>
+    <t>re-do introduction questions</t>
+  </si>
+  <si>
+    <t>Do 30 days of code each day</t>
+  </si>
+  <si>
+    <t>Do Problem Solving Question - Easy Everyday</t>
+  </si>
+  <si>
+    <t>Keep Repeating all questions everyday</t>
+  </si>
+  <si>
+    <t>Problem Solving</t>
+  </si>
+  <si>
+    <t>To pickup common methods to code</t>
+  </si>
+  <si>
+    <t>AlgoExpert and Leet Code Side by Side</t>
+  </si>
+  <si>
+    <t>Finish Doing all questions at Hacker Rank</t>
+  </si>
+  <si>
+    <t>Januray,2021 - Joma Class (Couple of months)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -163,13 +180,46 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -184,12 +234,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,45 +558,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48ACE8D-5980-5441-9666-6F36F07F6D8E}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.5" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.83203125" customWidth="1"/>
+    <col min="10" max="10" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1"/>
+      <c r="G1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="8"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>44116</v>
       </c>
@@ -556,10 +638,18 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>44114</v>
       </c>
@@ -573,10 +663,18 @@
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>44114</v>
       </c>
@@ -590,10 +688,18 @@
         <v>1</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44114</v>
       </c>
@@ -607,10 +713,18 @@
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44114</v>
       </c>
@@ -624,10 +738,10 @@
         <v>1</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44116</v>
       </c>
@@ -641,105 +755,138 @@
         <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>44115</v>
       </c>
       <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="2">
+        <v>44116</v>
+      </c>
+      <c r="G12" t="s">
         <v>26</v>
       </c>
-      <c r="C12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="H12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>44115</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>44116</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44116</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -762,137 +909,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EB890C2-6ADD-D344-8F4C-02F401BEA9C1}">
-  <dimension ref="A1:H27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5" customWidth="1"/>
-    <col min="8" max="8" width="31.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
-        <v>44144</v>
-      </c>
-      <c r="B25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
-        <v>44144</v>
-      </c>
-      <c r="B26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
-        <v>44144</v>
-      </c>
-      <c r="B27" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>